<commit_message>
Include Enum in sample for unit test
</commit_message>
<xml_diff>
--- a/test/Excel.IO.Test/Resources/test.xlsx
+++ b/test/Excel.IO.Test/Resources/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capre\Documents\dev\vsts\HCM-OnboardingService\src\OnboardingServiceTests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capre\Documents\dev\github\Excel-IO\test\Excel.IO.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBFAA31-F85B-449A-B048-ADB38D1720F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="5160" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
+    <workbookView xWindow="2033" yWindow="2512" windowWidth="16874" windowHeight="10523" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Age</t>
   </si>
@@ -157,6 +158,18 @@
   </si>
   <si>
     <t xml:space="preserve">109 somewhere st, somewhere, 12345 </t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CategoryA</t>
+  </si>
+  <si>
+    <t>CategoryC</t>
+  </si>
+  <si>
+    <t>CategoryB</t>
   </si>
 </sst>
 </file>
@@ -509,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3072FA3-C783-4C8B-A4CE-52D7109D9156}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -524,7 +537,7 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -546,8 +559,11 @@
       <c r="G1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -569,8 +585,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>43102</v>
       </c>
@@ -592,8 +611,11 @@
       <c r="G3">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>43103</v>
       </c>
@@ -615,8 +637,11 @@
       <c r="G4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>43104</v>
       </c>
@@ -638,8 +663,11 @@
       <c r="G5">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>43105</v>
       </c>
@@ -661,8 +689,11 @@
       <c r="G6">
         <v>523523</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>43106</v>
       </c>
@@ -684,8 +715,11 @@
       <c r="G7">
         <v>400</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>43107</v>
       </c>
@@ -707,8 +741,11 @@
       <c r="G8">
         <v>203</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>43108</v>
       </c>
@@ -730,8 +767,11 @@
       <c r="G9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>43109</v>
       </c>
@@ -753,8 +793,11 @@
       <c r="G10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>43110</v>
       </c>
@@ -775,6 +818,9 @@
       </c>
       <c r="G11">
         <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new tests Moved tests to ExcelConverterTests Fixed some ids causing incorrect data parses
</commit_message>
<xml_diff>
--- a/test/Excel.IO.Test/Resources/test.xlsx
+++ b/test/Excel.IO.Test/Resources/test.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capre\Documents\dev\github\Excel-IO\test\Excel.IO.Test\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoldenProjects\Excel-IO\test\Excel.IO.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBFAA31-F85B-449A-B048-ADB38D1720F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1DE2AA-6268-4435-BDB1-B0539F2489BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2033" yWindow="2512" windowWidth="16874" windowHeight="10523" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="69">
   <si>
     <t>Age</t>
   </si>
@@ -170,16 +180,103 @@
   </si>
   <si>
     <t>CategoryB</t>
+  </si>
+  <si>
+    <t>mail@mail.com</t>
+  </si>
+  <si>
+    <t>Category7</t>
+  </si>
+  <si>
+    <t>Category6</t>
+  </si>
+  <si>
+    <t>Category5</t>
+  </si>
+  <si>
+    <t>Category4</t>
+  </si>
+  <si>
+    <t>Category3</t>
+  </si>
+  <si>
+    <t>Category2</t>
+  </si>
+  <si>
+    <t>Category1</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>DayMonth</t>
+  </si>
+  <si>
+    <t>LongDate2</t>
+  </si>
+  <si>
+    <t>LongDate</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>ProbabilityOfSameAge</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>AgePercentage</t>
+  </si>
+  <si>
+    <t>HouseholdIncome</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>IsMarried</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="7">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-40C]mmmmm;@"/>
+    <numFmt numFmtId="165" formatCode="d/m;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="168" formatCode="[&lt;=999999999]###\ ###\ ###;\(###\)\ ###\ ###\ ###"/>
+    <numFmt numFmtId="169" formatCode="d/m/yy\ h:mm;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,15 +299,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -524,20 +639,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3072FA3-C783-4C8B-A4CE-52D7109D9156}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -563,7 +678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -589,7 +704,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43102</v>
       </c>
@@ -615,7 +730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43103</v>
       </c>
@@ -641,7 +756,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43104</v>
       </c>
@@ -667,7 +782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43105</v>
       </c>
@@ -693,7 +808,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43106</v>
       </c>
@@ -719,7 +834,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43107</v>
       </c>
@@ -745,7 +860,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43108</v>
       </c>
@@ -771,7 +886,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43109</v>
       </c>
@@ -797,7 +912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43110</v>
       </c>
@@ -837,9 +952,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -850,7 +965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -861,7 +976,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -872,7 +987,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -883,7 +998,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -898,4 +1013,1067 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC75D8B-FCC3-4FDD-BFA1-3492D5699A54}">
+  <dimension ref="A1:AC11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="29" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>43101.0625</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="13">
+        <v>25</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>351289086591</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9">
+        <f ca="1">RANDBETWEEN(1000,10000)</f>
+        <v>5644</v>
+      </c>
+      <c r="O2" s="8">
+        <f>(SUMIF(I2:I11,I2,I2:I11)/I2)/COUNT(I2:I11)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P2" s="7">
+        <v>29640</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>O3</f>
+        <v>0.3</v>
+      </c>
+      <c r="R2" s="5">
+        <f>6.62607*10^-34</f>
+        <v>6.6260700000000011E-34</v>
+      </c>
+      <c r="S2" s="4">
+        <v>31179</v>
+      </c>
+      <c r="T2" s="4">
+        <v>31920</v>
+      </c>
+      <c r="U2" s="3">
+        <v>43950</v>
+      </c>
+      <c r="V2" s="2">
+        <v>43950</v>
+      </c>
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>43102.449583333335</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="13">
+        <v>30</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12">
+        <v>351289124176</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="10">
+        <v>123</v>
+      </c>
+      <c r="N3" s="9">
+        <f ca="1">RANDBETWEEN(1000,10000)</f>
+        <v>5541</v>
+      </c>
+      <c r="O3" s="8">
+        <f>(SUMIF(I2:I11,I3,I2:I11)/I3)/COUNT(I2:I11)</f>
+        <v>0.3</v>
+      </c>
+      <c r="P3" s="7">
+        <v>29641</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>O3</f>
+        <v>0.3</v>
+      </c>
+      <c r="R3" s="5">
+        <f>3*10^-8</f>
+        <v>3.0000000000000004E-8</v>
+      </c>
+      <c r="S3" s="4">
+        <v>31180</v>
+      </c>
+      <c r="T3" s="4">
+        <v>31921</v>
+      </c>
+      <c r="U3" s="3">
+        <v>43951</v>
+      </c>
+      <c r="V3" s="2">
+        <v>43951</v>
+      </c>
+      <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <f>SUM(A2,365)</f>
+        <v>43466.0625</v>
+      </c>
+      <c r="B4">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="b">
+        <f>NOT(C3)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f>CHAR(98+1)</f>
+        <v>c</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <f>SUM(15,0.5)</f>
+        <v>15.5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="13">
+        <f>I3*2+4</f>
+        <v>64</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <f>351289776747+2</f>
+        <v>351289776749</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="10">
+        <f>SUM(15,0.5)</f>
+        <v>15.5</v>
+      </c>
+      <c r="N4" s="9">
+        <f ca="1">RANDBETWEEN(1000,10000)</f>
+        <v>9017</v>
+      </c>
+      <c r="O4" s="8">
+        <f>(SUMIF(I2:I11,I4,I2:I11)/I4)/COUNT(I2:I11)</f>
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="7">
+        <v>29642</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="R4" s="5">
+        <f>9.11*10^-31</f>
+        <v>9.1100000000000003E-31</v>
+      </c>
+      <c r="S4" s="4">
+        <v>31181</v>
+      </c>
+      <c r="T4" s="4">
+        <v>31922</v>
+      </c>
+      <c r="U4" s="3">
+        <v>43952</v>
+      </c>
+      <c r="V4" s="2">
+        <v>43952</v>
+      </c>
+      <c r="W4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>43104</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5">
+        <v>35</v>
+      </c>
+      <c r="H5" t="str">
+        <f>SUBSTITUTE(H4,"CategoryA","CategoryC")</f>
+        <v>CategoryC</v>
+      </c>
+      <c r="I5" s="13">
+        <v>35</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>351289238179</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="10">
+        <v>35</v>
+      </c>
+      <c r="N5" s="9">
+        <v>7278</v>
+      </c>
+      <c r="O5" s="8">
+        <f>0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="7">
+        <f>SUM(P4,1)</f>
+        <v>29643</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>O5+1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R5" s="5">
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S5" s="4">
+        <f>S4+1</f>
+        <v>31182</v>
+      </c>
+      <c r="T5" s="4">
+        <f>T4+1</f>
+        <v>31923</v>
+      </c>
+      <c r="U5" s="3">
+        <v>43953</v>
+      </c>
+      <c r="V5" s="2">
+        <v>43953</v>
+      </c>
+      <c r="W5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>43105</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6">
+        <v>523523</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="13">
+        <v>30</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12">
+        <v>351289922045</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="10">
+        <v>523523</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" ref="N6:N11" ca="1" si="0">RANDBETWEEN(1000,10000)</f>
+        <v>3185</v>
+      </c>
+      <c r="O6" s="8">
+        <f>(SUMIF(I2:I11,I6,I2:I11)/I6)/COUNT(I2:I11)</f>
+        <v>0.3</v>
+      </c>
+      <c r="P6" s="7">
+        <v>29644</v>
+      </c>
+      <c r="Q6" s="6">
+        <f t="shared" ref="Q6:Q11" si="1">O6</f>
+        <v>0.3</v>
+      </c>
+      <c r="R6" s="5">
+        <f>1.675*10^-27</f>
+        <v>1.6750000000000003E-27</v>
+      </c>
+      <c r="S6" s="4">
+        <v>31183</v>
+      </c>
+      <c r="T6" s="4">
+        <v>31924</v>
+      </c>
+      <c r="U6" s="3">
+        <f>U4+1</f>
+        <v>43953</v>
+      </c>
+      <c r="V6" s="2">
+        <v>43954</v>
+      </c>
+      <c r="W6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>43106</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="13">
+        <v>26</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>351289366581</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="10">
+        <v>400</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1963</v>
+      </c>
+      <c r="O7" s="8">
+        <f>(SUMIF(I2:I11,I7,I2:I11)/I7)/COUNT(I2:I11)</f>
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="7">
+        <v>29645</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="R7" s="5">
+        <f>1.673*10^-27</f>
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S7" s="4">
+        <v>31184</v>
+      </c>
+      <c r="T7" s="4">
+        <v>31925</v>
+      </c>
+      <c r="U7" s="3">
+        <v>43955</v>
+      </c>
+      <c r="V7" s="2">
+        <v>43955</v>
+      </c>
+      <c r="W7" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>43107</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>203</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="13">
+        <v>28</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>351289966202</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="10">
+        <v>203</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7905</v>
+      </c>
+      <c r="O8" s="8">
+        <f>(SUMIF(I2:I11,I8,I2:I11)/I8)/COUNT(I2:I11)</f>
+        <v>0.1</v>
+      </c>
+      <c r="P8" s="7">
+        <v>29646</v>
+      </c>
+      <c r="Q8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="R8" s="5">
+        <f>1.673*10^-27</f>
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S8" s="4">
+        <v>31185</v>
+      </c>
+      <c r="T8" s="4">
+        <v>31926</v>
+      </c>
+      <c r="U8" s="3">
+        <v>43956</v>
+      </c>
+      <c r="V8" s="2">
+        <v>43956</v>
+      </c>
+      <c r="W8" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>43108</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="13">
+        <v>25</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>351289922145</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="10">
+        <v>20</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4563</v>
+      </c>
+      <c r="O9" s="8">
+        <f>(SUMIF(I2:I11,I9,I2:I11)/I9)/COUNT(I2:I11)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P9" s="7">
+        <v>29647</v>
+      </c>
+      <c r="Q9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="R9" s="5">
+        <f>1.673*10^-27</f>
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S9" s="4">
+        <v>31186</v>
+      </c>
+      <c r="T9" s="4">
+        <v>31927</v>
+      </c>
+      <c r="U9" s="3">
+        <v>43957</v>
+      </c>
+      <c r="V9" s="2">
+        <v>43957</v>
+      </c>
+      <c r="W9" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>43109</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="13">
+        <v>30</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <v>351289922245</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="10">
+        <v>3</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>5420</v>
+      </c>
+      <c r="O10" s="8">
+        <f>(SUMIF(I2:I11,I10,I2:I11)/I10)/COUNT(I2:I11)</f>
+        <v>0.3</v>
+      </c>
+      <c r="P10" s="7">
+        <v>29648</v>
+      </c>
+      <c r="Q10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="R10" s="5">
+        <f>1.673*10^-27</f>
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S10" s="4">
+        <v>31187</v>
+      </c>
+      <c r="T10" s="4">
+        <v>31928</v>
+      </c>
+      <c r="U10" s="3">
+        <v>43958</v>
+      </c>
+      <c r="V10" s="2">
+        <v>43958</v>
+      </c>
+      <c r="W10" t="s">
+        <v>45</v>
+      </c>
+      <c r="X10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>43110</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="13">
+        <v>39</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>351289922345</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>6118</v>
+      </c>
+      <c r="O11" s="8">
+        <f>(SUMIF(I2:I11,I11,I2:I11)/I11)/COUNT(I2:I11)</f>
+        <v>0.1</v>
+      </c>
+      <c r="P11" s="7">
+        <v>29649</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="R11" s="5">
+        <f>1.673*10^-27</f>
+        <v>1.6730000000000002E-27</v>
+      </c>
+      <c r="S11" s="4">
+        <v>31188</v>
+      </c>
+      <c r="T11" s="4">
+        <v>31929</v>
+      </c>
+      <c r="U11" s="3">
+        <v>43959</v>
+      </c>
+      <c r="V11" s="2">
+        <v>43959</v>
+      </c>
+      <c r="W11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{D53EBB28-2AE9-4406-BBBB-B62247E8FAA9}"/>
+    <hyperlink ref="L3:L11" r:id="rId2" display="mail@mail.com" xr:uid="{7FAFE732-F407-4B54-B353-84714A37F820}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>